<commit_message>
Versão 1.3 - correção de bugs e README.md
</commit_message>
<xml_diff>
--- a/results/csv/resultados_accd_0001.xlsx
+++ b/results/csv/resultados_accd_0001.xlsx
@@ -31,172 +31,172 @@
     <t>sperman_coef</t>
   </si>
   <si>
-    <t>('RandomForest', (2.097826627243606, 0.7563509488032218))</t>
-  </si>
-  <si>
-    <t>('DecisionTree', (1.9298153055774196, 0.7563956332469395))</t>
-  </si>
-  <si>
-    <t>('Knn10', (1.9272747763699554, 0.7319053522713357))</t>
-  </si>
-  <si>
-    <t>('Knn5', (1.6866453831751222, 0.7128458097177036))</t>
-  </si>
-  <si>
-    <t>('LDA', (1.2377517514903504, 0.6753846338630222))</t>
-  </si>
-  <si>
-    <t>('Knn1', (1.0817749748269454, 0.6472733703791613))</t>
-  </si>
-  <si>
-    <t>('NaiveBayes', (0.14280361033808547, 0.5294468484269127))</t>
-  </si>
-  <si>
-    <t>('DecisionTree', (1.218342761284374, 0.7563956332469395))</t>
-  </si>
-  <si>
-    <t>('RandomForest', (1.1652332108771621, 0.7563509488032218))</t>
-  </si>
-  <si>
-    <t>('Knn10', (1.1104470637896706, 0.7319053522713357))</t>
-  </si>
-  <si>
-    <t>('Knn5', (1.0785604546908567, 0.7128458097177036))</t>
-  </si>
-  <si>
-    <t>('Knn1', (0.9314077313709658, 0.6472733703791613))</t>
-  </si>
-  <si>
-    <t>('LDA', (0.8939102031215063, 0.6753846338630222))</t>
-  </si>
-  <si>
-    <t>('NaiveBayes', (0.6380924560113563, 0.5294468484269127))</t>
-  </si>
-  <si>
-    <t>('DecisionTree', (1.2176536150778876, 0.7563956332469395))</t>
-  </si>
-  <si>
-    <t>('RandomForest', (1.2000016144772938, 0.7563509488032218))</t>
-  </si>
-  <si>
-    <t>('Knn10', (1.16741512182603, 0.7319053522713357))</t>
-  </si>
-  <si>
-    <t>('Knn5', (1.1191939000586475, 0.7128458097177036))</t>
-  </si>
-  <si>
-    <t>('Knn1', (0.9499165515879016, 0.6472733703791613))</t>
-  </si>
-  <si>
-    <t>('LDA', (0.9465995241492815, 0.6753846338630222))</t>
-  </si>
-  <si>
-    <t>('NaiveBayes', (0.5596470152409644, 0.5294468484269127))</t>
-  </si>
-  <si>
-    <t>('DecisionTree', (1.2178052520558766, 0.7563956332469395))</t>
-  </si>
-  <si>
-    <t>('RandomForest', (1.207089896401074, 0.7563509488032218))</t>
-  </si>
-  <si>
-    <t>('Knn10', (1.1606072599406818, 0.7319053522713357))</t>
-  </si>
-  <si>
-    <t>('Knn5', (1.1083417148852877, 0.7128458097177036))</t>
-  </si>
-  <si>
-    <t>('LDA', (0.9535308428600987, 0.6753846338630222))</t>
-  </si>
-  <si>
-    <t>('Knn1', (0.9306621958295106, 0.6472733703791613))</t>
-  </si>
-  <si>
-    <t>('NaiveBayes', (0.5807164780555469, 0.5294468484269127))</t>
-  </si>
-  <si>
-    <t>('DecisionTree', (1.203188308397493, 0.7563956332469395))</t>
-  </si>
-  <si>
-    <t>('RandomForest', (1.1944117589631935, 0.7563509488032218))</t>
-  </si>
-  <si>
-    <t>('Knn10', (1.1572479763821506, 0.7319053522713357))</t>
-  </si>
-  <si>
-    <t>('Knn5', (1.1157523628497725, 0.7128458097177036))</t>
-  </si>
-  <si>
-    <t>('Knn1', (0.9589691072508387, 0.6472733703791613))</t>
-  </si>
-  <si>
-    <t>('LDA', (0.9516762630863348, 0.6753846338630222))</t>
-  </si>
-  <si>
-    <t>('NaiveBayes', (0.5720582992735751, 0.5294468484269127))</t>
-  </si>
-  <si>
-    <t>('DecisionTree', (1.200459959596763, 0.7563956332469395))</t>
-  </si>
-  <si>
-    <t>('RandomForest', (1.1915375838610438, 0.7563509488032218))</t>
-  </si>
-  <si>
-    <t>('Knn10', (1.1541221643435429, 0.7319053522713357))</t>
-  </si>
-  <si>
-    <t>('Knn5', (1.100499389828484, 0.7128458097177036))</t>
-  </si>
-  <si>
-    <t>('LDA', (0.9451031703128743, 0.6753846338630222))</t>
-  </si>
-  <si>
-    <t>('Knn1', (0.9359198587439702, 0.6472733703791613))</t>
-  </si>
-  <si>
-    <t>('NaiveBayes', (0.6079400894092936, 0.5294468484269127))</t>
-  </si>
-  <si>
-    <t>('RandomForest', (0.96295663170451, 0.7563509488032218))</t>
-  </si>
-  <si>
-    <t>('Knn10', (0.9518048174253575, 0.7319053522713357))</t>
-  </si>
-  <si>
-    <t>('LDA', (0.9476196080010101, 0.6753846338630222))</t>
-  </si>
-  <si>
-    <t>('Knn5', (0.9091330605886366, 0.7128458097177036))</t>
-  </si>
-  <si>
-    <t>('DecisionTree', (0.9068975691488018, 0.7563956332469395))</t>
-  </si>
-  <si>
-    <t>('Knn1', (0.8194607973662728, 0.6472733703791613))</t>
-  </si>
-  <si>
-    <t>('NaiveBayes', (0.6819089389468507, 0.5294468484269127))</t>
-  </si>
-  <si>
-    <t>('DecisionTree', (1.2202379130506533, 0.7563956332469395))</t>
-  </si>
-  <si>
-    <t>('RandomForest', (1.2026819049022577, 0.7563509488032218))</t>
-  </si>
-  <si>
-    <t>('Knn10', (1.1531692375865465, 0.7319053522713357))</t>
-  </si>
-  <si>
-    <t>('Knn5', (1.1097561081057363, 0.7128458097177036))</t>
-  </si>
-  <si>
-    <t>('LDA', (0.9501686323588984, 0.6753846338630222))</t>
-  </si>
-  <si>
-    <t>('Knn1', (0.9481064902706642, 0.6472733703791613))</t>
-  </si>
-  <si>
-    <t>('NaiveBayes', (0.5704386811758076, 0.5294468484269127))</t>
+    <t>('RandomForest', (2.151429674410282, 0.7594959733070695))</t>
+  </si>
+  <si>
+    <t>('Knn10', (1.926330030521544, 0.7319053522713357))</t>
+  </si>
+  <si>
+    <t>('DecisionTree', (1.8917505570038493, 0.7540653475337438))</t>
+  </si>
+  <si>
+    <t>('Knn5', (1.6857194765779724, 0.7128458097177036))</t>
+  </si>
+  <si>
+    <t>('LDA', (1.2373644558632935, 0.6753846338630222))</t>
+  </si>
+  <si>
+    <t>('Knn1', (1.0809838643784946, 0.6472733703791613))</t>
+  </si>
+  <si>
+    <t>('NaiveBayes', (0.14278983669165277, 0.5294468484269127))</t>
+  </si>
+  <si>
+    <t>('DecisionTree', (1.2123171124514067, 0.7540653475337438))</t>
+  </si>
+  <si>
+    <t>('RandomForest', (1.1719507301248393, 0.7594959733070695))</t>
+  </si>
+  <si>
+    <t>('Knn10', (1.1107397792349358, 0.7319053522713357))</t>
+  </si>
+  <si>
+    <t>('Knn5', (1.078780913976465, 0.7128458097177036))</t>
+  </si>
+  <si>
+    <t>('Knn1', (0.9315950378153693, 0.6472733703791613))</t>
+  </si>
+  <si>
+    <t>('LDA', (0.8942340309054552, 0.6753846338630222))</t>
+  </si>
+  <si>
+    <t>('NaiveBayes', (0.6387237856126603, 0.5294468484269127))</t>
+  </si>
+  <si>
+    <t>('DecisionTree', (1.2113278699772818, 0.7540653475337438))</t>
+  </si>
+  <si>
+    <t>('RandomForest', (1.2102631078639372, 0.7594959733070695))</t>
+  </si>
+  <si>
+    <t>('Knn10', (1.1672089703031432, 0.7319053522713357))</t>
+  </si>
+  <si>
+    <t>('Knn5', (1.1190590580108295, 0.7128458097177036))</t>
+  </si>
+  <si>
+    <t>('Knn1', (0.9497811465864677, 0.6472733703791613))</t>
+  </si>
+  <si>
+    <t>('LDA', (0.9464924661090054, 0.6753846338630222))</t>
+  </si>
+  <si>
+    <t>('NaiveBayes', (0.5600623026359991, 0.5294468484269127))</t>
+  </si>
+  <si>
+    <t>('RandomForest', (1.2170645838379592, 0.7594959733070695))</t>
+  </si>
+  <si>
+    <t>('DecisionTree', (1.2117369461265741, 0.7540653475337438))</t>
+  </si>
+  <si>
+    <t>('Knn10', (1.1603714022565117, 0.7319053522713357))</t>
+  </si>
+  <si>
+    <t>('Knn5', (1.1082003281710633, 0.7128458097177036))</t>
+  </si>
+  <si>
+    <t>('LDA', (0.9534094428581625, 0.6753846338630222))</t>
+  </si>
+  <si>
+    <t>('Knn1', (0.9305341827483555, 0.6472733703791613))</t>
+  </si>
+  <si>
+    <t>('NaiveBayes', (0.5811958730176384, 0.5294468484269127))</t>
+  </si>
+  <si>
+    <t>('RandomForest', (1.2048538766631265, 0.7594959733070695))</t>
+  </si>
+  <si>
+    <t>('DecisionTree', (1.1962394900874063, 0.7540653475337438))</t>
+  </si>
+  <si>
+    <t>('Knn10', (1.1571285853165822, 0.7319053522713357))</t>
+  </si>
+  <si>
+    <t>('Knn5', (1.1157091386800295, 0.7128458097177036))</t>
+  </si>
+  <si>
+    <t>('Knn1', (0.9589110498353272, 0.6472733703791613))</t>
+  </si>
+  <si>
+    <t>('LDA', (0.9516994161223318, 0.6753846338630222))</t>
+  </si>
+  <si>
+    <t>('NaiveBayes', (0.5724149429815409, 0.5294468484269127))</t>
+  </si>
+  <si>
+    <t>('RandomForest', (1.20142055609216, 0.7594959733070695))</t>
+  </si>
+  <si>
+    <t>('DecisionTree', (1.1942612738535803, 0.7540653475337438))</t>
+  </si>
+  <si>
+    <t>('Knn10', (1.1539285184560222, 0.7319053522713357))</t>
+  </si>
+  <si>
+    <t>('Knn5', (1.1003799029232246, 0.7128458097177036))</t>
+  </si>
+  <si>
+    <t>('LDA', (0.9450467796729798, 0.6753846338630222))</t>
+  </si>
+  <si>
+    <t>('Knn1', (0.9358041383162409, 0.6472733703791613))</t>
+  </si>
+  <si>
+    <t>('NaiveBayes', (0.6084430371476631, 0.5294468484269127))</t>
+  </si>
+  <si>
+    <t>('RandomForest', (0.9714381179467713, 0.7594959733070695))</t>
+  </si>
+  <si>
+    <t>('Knn10', (0.9516558424331265, 0.7319053522713357))</t>
+  </si>
+  <si>
+    <t>('LDA', (0.947583130314012, 0.6753846338630222))</t>
+  </si>
+  <si>
+    <t>('Knn5', (0.9090488404151519, 0.7128458097177036))</t>
+  </si>
+  <si>
+    <t>('DecisionTree', (0.9013743553037171, 0.7540653475337438))</t>
+  </si>
+  <si>
+    <t>('Knn1', (0.8193326396879507, 0.6472733703791613))</t>
+  </si>
+  <si>
+    <t>('NaiveBayes', (0.6823967374042752, 0.5294468484269127))</t>
+  </si>
+  <si>
+    <t>('DecisionTree', (1.2202819478702798, 0.7540653475337438))</t>
+  </si>
+  <si>
+    <t>('RandomForest', (1.2074433108774394, 0.7594959733070695))</t>
+  </si>
+  <si>
+    <t>('Knn10', (1.1524296008964432, 0.7319053522713357))</t>
+  </si>
+  <si>
+    <t>('Knn5', (1.109078419726502, 0.7128458097177036))</t>
+  </si>
+  <si>
+    <t>('LDA', (0.9495932130840735, 0.6753846338630222))</t>
+  </si>
+  <si>
+    <t>('Knn1', (0.9475446232632139, 0.6472733703791613))</t>
+  </si>
+  <si>
+    <t>('NaiveBayes', (0.5704556562012737, 0.5294468484269127))</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -596,7 +596,7 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -610,7 +610,7 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -624,7 +624,7 @@
         <v>13</v>
       </c>
       <c r="D5">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="D6">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -652,7 +652,7 @@
         <v>15</v>
       </c>
       <c r="D7">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -666,7 +666,7 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +704,7 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -718,7 +718,7 @@
         <v>18</v>
       </c>
       <c r="D3">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -732,7 +732,7 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -746,7 +746,7 @@
         <v>20</v>
       </c>
       <c r="D5">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -760,7 +760,7 @@
         <v>21</v>
       </c>
       <c r="D6">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -774,7 +774,7 @@
         <v>22</v>
       </c>
       <c r="D7">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -788,7 +788,7 @@
         <v>23</v>
       </c>
       <c r="D8">
-        <v>0.9285714285714286</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
   </sheetData>
@@ -1192,7 +1192,7 @@
         <v>45</v>
       </c>
       <c r="D2">
-        <v>0.75</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1206,7 +1206,7 @@
         <v>46</v>
       </c>
       <c r="D3">
-        <v>0.75</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1220,7 +1220,7 @@
         <v>47</v>
       </c>
       <c r="D4">
-        <v>0.75</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1234,7 +1234,7 @@
         <v>48</v>
       </c>
       <c r="D5">
-        <v>0.75</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1248,7 +1248,7 @@
         <v>49</v>
       </c>
       <c r="D6">
-        <v>0.75</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1262,7 +1262,7 @@
         <v>50</v>
       </c>
       <c r="D7">
-        <v>0.75</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1276,7 +1276,7 @@
         <v>51</v>
       </c>
       <c r="D8">
-        <v>0.75</v>
+        <v>0.8571428571428572</v>
       </c>
     </row>
   </sheetData>
@@ -1314,7 +1314,7 @@
         <v>52</v>
       </c>
       <c r="D2">
-        <v>0.9642857142857143</v>
+        <v>0.8928571428571429</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1328,7 +1328,7 @@
         <v>53</v>
       </c>
       <c r="D3">
-        <v>0.9642857142857143</v>
+        <v>0.8928571428571429</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1342,7 +1342,7 @@
         <v>54</v>
       </c>
       <c r="D4">
-        <v>0.9642857142857143</v>
+        <v>0.8928571428571429</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1356,7 +1356,7 @@
         <v>55</v>
       </c>
       <c r="D5">
-        <v>0.9642857142857143</v>
+        <v>0.8928571428571429</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1370,7 +1370,7 @@
         <v>56</v>
       </c>
       <c r="D6">
-        <v>0.9642857142857143</v>
+        <v>0.8928571428571429</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1384,7 +1384,7 @@
         <v>57</v>
       </c>
       <c r="D7">
-        <v>0.9642857142857143</v>
+        <v>0.8928571428571429</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1398,7 +1398,7 @@
         <v>58</v>
       </c>
       <c r="D8">
-        <v>0.9642857142857143</v>
+        <v>0.8928571428571429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>